<commit_message>
Johns main reaction changes
</commit_message>
<xml_diff>
--- a/Matt_Work/Genes from Genome Paper/sorted missing genes.xlsx
+++ b/Matt_Work/Genes from Genome Paper/sorted missing genes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="96" windowWidth="10500" windowHeight="9264" activeTab="1"/>
+    <workbookView xWindow="384" yWindow="96" windowWidth="10500" windowHeight="9264" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Non-Metabolic" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="107">
   <si>
     <t>Transcription</t>
   </si>
@@ -315,7 +315,28 @@
     <t>mmp0200,0508,1691</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Proposed Rxn</t>
+  </si>
+  <si>
+    <t>HdrABC</t>
+  </si>
+  <si>
+    <t>rxn03127_c0</t>
+  </si>
+  <si>
+    <t>rxn06299_c0</t>
+  </si>
+  <si>
+    <t>rxn00371_c0</t>
+  </si>
+  <si>
+    <t>CODH</t>
+  </si>
+  <si>
+    <t>rxn11938_c0</t>
+  </si>
+  <si>
+    <t>Ehb</t>
   </si>
 </sst>
 </file>
@@ -331,12 +352,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -351,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -361,6 +388,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,10 +873,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -990,28 +1018,6 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" t="s">
-        <v>58</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1019,144 +1025,198 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="101.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="157.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="18.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="157.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>79</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
         <v>83</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" t="s">
         <v>87</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
         <v>90</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" t="s">
         <v>91</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" t="s">
         <v>83</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
         <v>94</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" t="s">
         <v>87</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="s">
-        <v>99</v>
+    <row r="12" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Alanine, GOGAT, added NADNADP codes
</commit_message>
<xml_diff>
--- a/Matt_Work/Genes from Genome Paper/sorted missing genes.xlsx
+++ b/Matt_Work/Genes from Genome Paper/sorted missing genes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="96" windowWidth="10500" windowHeight="9264" activeTab="2"/>
+    <workbookView xWindow="384" yWindow="156" windowWidth="10500" windowHeight="9204" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Non-Metabolic" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
   <si>
     <t>Transcription</t>
   </si>
@@ -210,9 +210,6 @@
     <t>mmp0819</t>
   </si>
   <si>
-    <t>Vhc; non-F420 reducing hydrogenases</t>
-  </si>
-  <si>
     <t>mmp0977</t>
   </si>
   <si>
@@ -222,9 +219,6 @@
     <t>mmp1383</t>
   </si>
   <si>
-    <t>Vhu; non-F420 reducing hydrogenases</t>
-  </si>
-  <si>
     <t>mmp0821-0824</t>
   </si>
   <si>
@@ -337,13 +331,16 @@
   </si>
   <si>
     <t>Ehb</t>
+  </si>
+  <si>
+    <t>rxn00260_c0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,19 +348,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -381,14 +379,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,178 +691,179 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="D21" sqref="D21:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
         <v>9</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="4">
         <v>13</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -875,351 +874,421 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C3" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" t="s">
-        <v>58</v>
-      </c>
-    </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="157.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="129.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>58</v>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>